<commit_message>
Updated vehicle trip rate and average one-way vehicle trip length based on model runs done on Sept 22
</commit_message>
<xml_diff>
--- a/off_model_calculators/sandag_inputs/avg_vtrip_rates_length_CBTP_off_model_calc.xlsx
+++ b/off_model_calculators/sandag_inputs/avg_vtrip_rates_length_CBTP_off_model_calc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\RTP\2019RP\rp19_scen\analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\RES\TransModel\2019RTP\off_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D38F2EAF-84B4-4168-9C73-D2E8F6F3F59B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3E0B7F90-EE32-4D07-ABA9-2B4BEA9FE00D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="9330" xr2:uid="{AF09D215-C8DF-4848-A451-739E06982087}"/>
   </bookViews>
@@ -58,7 +58,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,16 +85,308 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -99,18 +394,223 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="47" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="50">
+    <cellStyle name="20% - Accent1" xfId="10" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="14" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="18" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="22" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="26" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="30" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="11" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="19" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="23" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="27" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="31" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="12" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="16" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="20" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="24" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="28" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="32" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="9" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="13" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="17" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="21" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="25" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="29" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="6" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="Explanatory Text 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="Heading 2 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Heading 3 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Heading 4 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Input" xfId="4" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 3" xfId="40" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="Normal 4" xfId="47" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="Normal 5" xfId="39" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="Normal 6" xfId="48" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="Normal 7" xfId="46" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="Note" xfId="8" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="5" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent 2" xfId="49" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="Title 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Total 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Warning Text 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -425,7 +925,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,25 +965,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C2" s="3">
-        <v>82</v>
-      </c>
-      <c r="D2">
-        <v>81</v>
+        <v>101</v>
+      </c>
+      <c r="D2" s="3">
+        <v>102</v>
       </c>
       <c r="E2" s="3">
-        <v>76</v>
+        <v>109</v>
       </c>
       <c r="F2" s="3">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="G2" s="3">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="H2" s="3">
-        <v>78</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -494,22 +994,22 @@
         <v>7.8807710000000002</v>
       </c>
       <c r="C3" s="1">
-        <v>7.8562630000000002</v>
-      </c>
-      <c r="D3">
-        <v>7.7965619999999998</v>
+        <v>7.8497079999999997</v>
+      </c>
+      <c r="D3" s="1">
+        <v>7.7908210000000002</v>
       </c>
       <c r="E3" s="1">
-        <v>7.6091129999999998</v>
+        <v>7.5972059999999999</v>
       </c>
       <c r="F3" s="1">
-        <v>7.5984080000000001</v>
+        <v>7.5925269999999996</v>
       </c>
       <c r="G3" s="1">
-        <v>7.3506309999999999</v>
+        <v>7.3438489999999996</v>
       </c>
       <c r="H3" s="1">
-        <v>7.5690710000000001</v>
+        <v>7.5609440000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -520,22 +1020,22 @@
         <v>7.1884079999999999</v>
       </c>
       <c r="C4" s="1">
-        <v>7.0709140000000001</v>
+        <v>7.0701150000000004</v>
       </c>
       <c r="D4" s="1">
-        <v>7.0202210000000003</v>
+        <v>7.0206860000000004</v>
       </c>
       <c r="E4" s="1">
-        <v>7.0742289999999999</v>
+        <v>7.079243</v>
       </c>
       <c r="F4" s="1">
-        <v>7.0260290000000003</v>
+        <v>7.0324660000000003</v>
       </c>
       <c r="G4" s="1">
-        <v>6.8323330000000002</v>
+        <v>6.8360779999999997</v>
       </c>
       <c r="H4" s="1">
-        <v>7.0291969999999999</v>
+        <v>7.032165</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>